<commit_message>
Prepare qlearning penalty rfs half day simulation
</commit_message>
<xml_diff>
--- a/output/exp14_hyperparam_tuning_2/stats_departDelay.xlsx
+++ b/output/exp14_hyperparam_tuning_2/stats_departDelay.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\I844141\Documents\Unisinos\2019-2\TCCII\workspace\TCC-II\output\exp14_hyperparam_tuning_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BACB36D4-5C33-4DC7-AFD3-385D75AAE2BF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF7A51DE-CD4D-46E2-ACD0-DA62AEE3618A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24360" yWindow="5985" windowWidth="17280" windowHeight="8970"/>
+    <workbookView xWindow="-3624" yWindow="7332" windowWidth="12300" windowHeight="6348" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="stats_departDelay" sheetId="1" r:id="rId1"/>
@@ -88,7 +88,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -614,19 +614,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <b/>
@@ -942,17 +930,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:W6"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="50.21875" customWidth="1"/>
-    <col min="2" max="21" width="0" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="46.77734375" customWidth="1"/>
+    <col min="2" max="17" width="0" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="12.33203125" customWidth="1"/>
+    <col min="19" max="19" width="8.88671875" customWidth="1"/>
+    <col min="20" max="20" width="7.21875" customWidth="1"/>
+    <col min="21" max="21" width="7.6640625" customWidth="1"/>
     <col min="22" max="22" width="15.44140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1828,7 +1820,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:Y12">
-    <cfRule type="expression" dxfId="1" priority="3">
+    <cfRule type="expression" dxfId="0" priority="3">
       <formula>B3=MIN(B$3:B$12)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1843,5 +1835,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>